<commit_message>
[+] Sse2 unrolec with intrinsic counter class, unit test
[+] add new unit tests
[*] fix bugs in classes
</commit_message>
<xml_diff>
--- a/calculation.xlsx
+++ b/calculation.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,12 +36,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -55,8 +62,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -337,25 +345,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:AQ41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F1" sqref="F1:AQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <v>2</v>
+      </c>
+      <c r="H1">
+        <v>3</v>
+      </c>
+      <c r="I1">
+        <v>4</v>
+      </c>
+      <c r="J1">
+        <v>5</v>
+      </c>
+      <c r="K1">
+        <v>6</v>
+      </c>
+      <c r="L1">
+        <v>7</v>
+      </c>
+      <c r="M1">
+        <v>8</v>
+      </c>
+      <c r="N1">
+        <v>9</v>
+      </c>
+      <c r="O1">
+        <v>1</v>
+      </c>
+      <c r="P1">
+        <v>2</v>
+      </c>
+      <c r="Q1">
+        <v>3</v>
+      </c>
+      <c r="R1">
+        <v>4</v>
+      </c>
+      <c r="S1">
+        <v>5</v>
+      </c>
+      <c r="T1">
+        <v>6</v>
+      </c>
+      <c r="U1">
+        <v>7</v>
+      </c>
+      <c r="V1">
+        <v>8</v>
+      </c>
+      <c r="W1">
+        <v>9</v>
+      </c>
+      <c r="X1">
+        <v>3</v>
+      </c>
+      <c r="Y1">
+        <v>5</v>
+      </c>
+      <c r="Z1">
+        <v>7</v>
+      </c>
+      <c r="AA1">
+        <v>9</v>
+      </c>
+      <c r="AB1">
+        <v>11</v>
+      </c>
+      <c r="AC1">
+        <v>13</v>
+      </c>
+      <c r="AD1">
+        <v>15</v>
+      </c>
+      <c r="AE1">
+        <v>17</v>
+      </c>
+      <c r="AF1">
+        <v>19</v>
+      </c>
+      <c r="AG1">
+        <v>21</v>
+      </c>
+      <c r="AH1">
+        <v>23</v>
+      </c>
+      <c r="AI1">
+        <v>3</v>
+      </c>
+      <c r="AJ1">
+        <v>4</v>
+      </c>
+      <c r="AK1">
+        <v>5</v>
+      </c>
+      <c r="AL1">
+        <v>6</v>
+      </c>
+      <c r="AM1">
+        <v>6</v>
+      </c>
+      <c r="AN1">
+        <v>8</v>
+      </c>
+      <c r="AO1">
+        <v>10</v>
+      </c>
+      <c r="AP1">
+        <v>12</v>
+      </c>
+      <c r="AQ1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <v>6.2</v>
+      </c>
+      <c r="L2">
+        <v>5.4</v>
+      </c>
+      <c r="M2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="N2">
+        <v>3.8</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <v>4</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2">
+        <v>6</v>
+      </c>
+      <c r="S2">
+        <v>7</v>
+      </c>
+      <c r="T2">
+        <v>6.6</v>
+      </c>
+      <c r="U2">
+        <v>6.4</v>
+      </c>
+      <c r="V2">
+        <v>6.4</v>
+      </c>
+      <c r="W2">
+        <v>6.6</v>
+      </c>
+      <c r="X2">
+        <v>7</v>
+      </c>
+      <c r="Y2">
+        <v>9</v>
+      </c>
+      <c r="Z2">
+        <v>11</v>
+      </c>
+      <c r="AA2">
+        <v>13</v>
+      </c>
+      <c r="AB2">
+        <v>15</v>
+      </c>
+      <c r="AC2">
+        <v>17</v>
+      </c>
+      <c r="AD2">
+        <v>19</v>
+      </c>
+      <c r="AE2">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -363,17 +563,23 @@
         <f>($A1+$A2+$A3+$A4+$A5)/5</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B16" si="0">($A2+$A3+$A4+$A5+$A6)/5</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" ref="B4:B15" si="0">($A2+$A3+$A4+$A5+$A6)/5</f>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -381,8 +587,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -390,8 +599,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -399,8 +611,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -408,8 +623,11 @@
         <f t="shared" si="0"/>
         <v>6.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -417,8 +635,11 @@
         <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -426,8 +647,11 @@
         <f t="shared" si="0"/>
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -435,8 +659,11 @@
         <f t="shared" si="0"/>
         <v>3.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -444,8 +671,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -453,8 +683,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -462,8 +695,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -471,8 +707,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
@@ -480,15 +719,660 @@
         <f>($A14+$A15+$A16+$A17+$A18)/5</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f t="shared" ref="B17:B39" si="1">($A15+$A16+$A17+$A18+$A19)/5</f>
+        <v>6.6</v>
+      </c>
+      <c r="C17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>6.4</v>
+      </c>
+      <c r="C18" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>6.4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>6.6</v>
+      </c>
+      <c r="C20" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>13</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C24" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C25" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="C26" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="C27" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="1"/>
+        <v>16.600000000000001</v>
+      </c>
+      <c r="C28" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>23</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="1"/>
+        <v>11.2</v>
+      </c>
+      <c r="C30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="1"/>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="1"/>
+        <v>4.8</v>
+      </c>
+      <c r="C32" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>5.8</v>
+      </c>
+      <c r="C33" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C34" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="1"/>
+        <v>8.4</v>
+      </c>
+      <c r="C35" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>10</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C36" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>16</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AO3"/>
+  <sheetViews>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3:AJ3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>1</v>
+      </c>
+      <c r="K1">
+        <v>2</v>
+      </c>
+      <c r="L1">
+        <v>3</v>
+      </c>
+      <c r="M1">
+        <v>4</v>
+      </c>
+      <c r="N1">
+        <v>5</v>
+      </c>
+      <c r="O1">
+        <v>6</v>
+      </c>
+      <c r="P1">
+        <v>7</v>
+      </c>
+      <c r="Q1">
+        <v>8</v>
+      </c>
+      <c r="R1">
+        <v>9</v>
+      </c>
+      <c r="S1">
+        <v>3</v>
+      </c>
+      <c r="T1">
+        <v>5</v>
+      </c>
+      <c r="U1">
+        <v>7</v>
+      </c>
+      <c r="V1">
+        <v>9</v>
+      </c>
+      <c r="W1">
+        <v>11</v>
+      </c>
+      <c r="X1">
+        <v>13</v>
+      </c>
+      <c r="Y1">
+        <v>15</v>
+      </c>
+      <c r="Z1">
+        <v>17</v>
+      </c>
+      <c r="AA1">
+        <v>19</v>
+      </c>
+      <c r="AB1">
+        <v>21</v>
+      </c>
+      <c r="AC1">
+        <v>23</v>
+      </c>
+      <c r="AD1">
+        <v>3</v>
+      </c>
+      <c r="AE1">
+        <v>4</v>
+      </c>
+      <c r="AF1">
+        <v>5</v>
+      </c>
+      <c r="AG1">
+        <v>6</v>
+      </c>
+      <c r="AH1">
+        <v>6</v>
+      </c>
+      <c r="AI1">
+        <v>8</v>
+      </c>
+      <c r="AJ1">
+        <v>10</v>
+      </c>
+      <c r="AK1">
+        <v>12</v>
+      </c>
+      <c r="AL1">
+        <v>14</v>
+      </c>
+      <c r="AM1">
+        <v>16</v>
+      </c>
+      <c r="AN1">
+        <v>18</v>
+      </c>
+      <c r="AO1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>6.2</v>
+      </c>
+      <c r="I2">
+        <v>5.4</v>
+      </c>
+      <c r="J2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K2">
+        <v>3.8</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>6</v>
+      </c>
+      <c r="P2">
+        <v>7</v>
+      </c>
+      <c r="Q2">
+        <v>6.6</v>
+      </c>
+      <c r="R2">
+        <v>6.4</v>
+      </c>
+      <c r="S2">
+        <v>6.4</v>
+      </c>
+      <c r="T2">
+        <v>6.6</v>
+      </c>
+      <c r="U2">
+        <v>7</v>
+      </c>
+      <c r="V2">
+        <v>9</v>
+      </c>
+      <c r="W2">
+        <v>11</v>
+      </c>
+      <c r="X2">
+        <v>13</v>
+      </c>
+      <c r="Y2">
+        <v>15</v>
+      </c>
+      <c r="Z2">
+        <v>17</v>
+      </c>
+      <c r="AA2">
+        <v>19</v>
+      </c>
+      <c r="AB2">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="AC2">
+        <v>14</v>
+      </c>
+      <c r="AD2">
+        <v>11.2</v>
+      </c>
+      <c r="AE2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AF2">
+        <v>4.8</v>
+      </c>
+      <c r="AG2">
+        <v>5.8</v>
+      </c>
+      <c r="AH2">
+        <v>7</v>
+      </c>
+      <c r="AI2">
+        <v>8.4</v>
+      </c>
+      <c r="AJ2">
+        <v>10</v>
+      </c>
+      <c r="AK2">
+        <v>12</v>
+      </c>
+      <c r="AL2">
+        <v>14</v>
+      </c>
+      <c r="AM2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>11</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3">
+        <v>13</v>
+      </c>
+      <c r="P3" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>15</v>
+      </c>
+      <c r="R3" s="1">
+        <v>16</v>
+      </c>
+      <c r="S3" s="1">
+        <v>17</v>
+      </c>
+      <c r="T3" s="1">
+        <v>18</v>
+      </c>
+      <c r="U3">
+        <v>19</v>
+      </c>
+      <c r="V3">
+        <v>20</v>
+      </c>
+      <c r="W3">
+        <v>21</v>
+      </c>
+      <c r="X3" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC3">
+        <v>27</v>
+      </c>
+      <c r="AD3">
+        <v>28</v>
+      </c>
+      <c r="AE3">
+        <v>29</v>
+      </c>
+      <c r="AF3">
+        <v>30</v>
+      </c>
+      <c r="AG3">
+        <v>31</v>
+      </c>
+      <c r="AH3">
+        <v>32</v>
+      </c>
+      <c r="AI3">
+        <v>33</v>
+      </c>
+      <c r="AJ3">
+        <v>34</v>
+      </c>
+      <c r="AK3">
+        <v>35</v>
+      </c>
+      <c r="AL3">
+        <v>36</v>
+      </c>
+      <c r="AM3">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[*] fix Sse2 supported class
</commit_message>
<xml_diff>
--- a/calculation.xlsx
+++ b/calculation.xlsx
@@ -347,8 +347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:AQ1"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AN1" activeCellId="1" sqref="F1:AQ1 AN1:AO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +553,30 @@
       </c>
       <c r="AE2">
         <v>16.600000000000001</v>
+      </c>
+      <c r="AF2">
+        <v>14</v>
+      </c>
+      <c r="AG2">
+        <v>11.2</v>
+      </c>
+      <c r="AH2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AI2">
+        <v>4.8</v>
+      </c>
+      <c r="AJ2">
+        <v>5.8</v>
+      </c>
+      <c r="AK2">
+        <v>7</v>
+      </c>
+      <c r="AL2">
+        <v>8.4</v>
+      </c>
+      <c r="AM2">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">

</xml_diff>